<commit_message>
add snmp commit command
</commit_message>
<xml_diff>
--- a/src/main/resources/SNMP/MibHolder.xlsx
+++ b/src/main/resources/SNMP/MibHolder.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="261">
   <si>
     <t>OID</t>
   </si>
@@ -805,6 +805,15 @@
   </si>
   <si>
     <t>.1.3.6.1.4.1.17713.20.2.3.1.1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pmpDevCpeLteBandCommit </t>
+  </si>
+  <si>
+    <t>.1.3.6.1.4.1.17713.20.2.3.1.2.15.0</t>
+  </si>
+  <si>
+    <t>commit</t>
   </si>
 </sst>
 </file>
@@ -4742,10 +4751,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4846,89 +4855,89 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>171</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>86</v>
+      <c r="A13" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>86</v>
@@ -4936,13 +4945,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>86</v>
@@ -4950,13 +4959,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>86</v>
@@ -4964,13 +4973,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>86</v>
@@ -4978,13 +4987,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>86</v>
@@ -4992,13 +5001,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>86</v>
@@ -5006,13 +5015,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>86</v>
@@ -5020,13 +5029,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>86</v>
@@ -5034,13 +5043,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>86</v>
@@ -5048,13 +5057,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>86</v>
@@ -5062,13 +5071,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>86</v>
@@ -5076,13 +5085,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>86</v>
@@ -5090,13 +5099,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>86</v>
@@ -5104,13 +5113,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>86</v>
@@ -5118,13 +5127,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>86</v>
@@ -5132,13 +5141,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>86</v>
@@ -5146,13 +5155,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>86</v>
@@ -5160,13 +5169,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>86</v>
@@ -5174,13 +5183,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>86</v>
@@ -5188,13 +5197,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>86</v>
@@ -5202,13 +5211,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>86</v>
@@ -5216,15 +5225,29 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update ANR MC scenario and MIBHolder
</commit_message>
<xml_diff>
--- a/src/main/resources/SNMP/MibHolder.xlsx
+++ b/src/main/resources/SNMP/MibHolder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="ENODEB_R15_00" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="269">
   <si>
     <t>OID</t>
   </si>
@@ -831,16 +831,16 @@
     <t>nghRemoveThreshold</t>
   </si>
   <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.23.1.33.40</t>
-  </si>
-  <si>
     <t>asLteStkCellAnrCfgNghRemoveThresholdCell1</t>
   </si>
   <si>
     <t>asLteStkCellAnrCfgNghRemoveThresholdCell2</t>
   </si>
   <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.23.1.33.41</t>
+    <t>1.3.6.1.4.1.989.1.20.1.4.23.1.33.40</t>
+  </si>
+  <si>
+    <t>1.3.6.1.4.1.989.1.20.1.4.23.1.33.41</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,6 +1808,34 @@
         <v>164</v>
       </c>
     </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="B52" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B53" t="s">
+        <v>268</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1816,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A52" sqref="A52:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,6 +2432,34 @@
       </c>
       <c r="D51" s="5" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="B52" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B53" t="s">
+        <v>268</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3005,10 +3061,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B52" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>264</v>
@@ -3019,7 +3075,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B53" t="s">
         <v>268</v>
@@ -3631,10 +3687,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B52" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>264</v>
@@ -3645,7 +3701,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B53" t="s">
         <v>268</v>
@@ -3667,13 +3723,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A53" sqref="A53:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -4255,7 +4311,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>165</v>
       </c>
@@ -4271,10 +4327,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B53" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>264</v>
@@ -4285,7 +4341,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B54" t="s">
         <v>268</v>
@@ -4307,8 +4363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4897,10 +4953,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B52" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>264</v>
@@ -4911,7 +4967,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B53" t="s">
         <v>268</v>

</xml_diff>

<commit_message>
add TX Power change to TCP_TP scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/SNMP/MibHolder.xlsx
+++ b/src/main/resources/SNMP/MibHolder.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spuser.AIRSPAN\git\Testspan_Runners\src\main\resources\SNMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sitshakov\git\Testspan_Runners\src\main\resources\SNMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ENODEB_R15_00" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="293">
   <si>
     <t>OID</t>
   </si>
@@ -901,6 +901,18 @@
   </si>
   <si>
     <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.20.40.174</t>
+  </si>
+  <si>
+    <t>1.3.6.1.4.1.989.1.20.1.4.1.1.16.40</t>
+  </si>
+  <si>
+    <t>1.3.6.1.4.1.989.1.20.1.4.1.1.16.41</t>
+  </si>
+  <si>
+    <t>asLteStkCellCfgTxPowerCell1</t>
+  </si>
+  <si>
+    <t>asLteStkCellCfgTxPowerCell2</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -2529,10 +2541,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD53"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,7 +3117,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>165</v>
       </c>
@@ -3144,6 +3156,34 @@
         <v>264</v>
       </c>
       <c r="D53" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B54" t="s">
+        <v>289</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B55" t="s">
+        <v>290</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3155,10 +3195,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD53"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3773,6 +3813,34 @@
         <v>86</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B54" t="s">
+        <v>289</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B55" t="s">
+        <v>290</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3781,10 +3849,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:XFD54"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4413,6 +4481,34 @@
         <v>86</v>
       </c>
     </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B55" t="s">
+        <v>289</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B56" t="s">
+        <v>290</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4421,10 +4517,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD53"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5036,6 +5132,34 @@
         <v>264</v>
       </c>
       <c r="D53" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B54" t="s">
+        <v>289</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B55" t="s">
+        <v>290</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update MibHolder file - add AutoPCI mib
</commit_message>
<xml_diff>
--- a/src/main/resources/SNMP/MibHolder.xlsx
+++ b/src/main/resources/SNMP/MibHolder.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spuser.AIRSPAN\git\Testspan_Runners\src\main\resources\SNMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sitshakov\git\Testspan_Runners\src\main\resources\SNMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ENODEB_R15_00" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="297">
   <si>
     <t>OID</t>
   </si>
@@ -922,6 +922,9 @@
   </si>
   <si>
     <t>Gemtek</t>
+  </si>
+  <si>
+    <t>PCI</t>
   </si>
 </sst>
 </file>
@@ -3204,10 +3207,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD55"/>
+      <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3850,6 +3853,20 @@
         <v>86</v>
       </c>
     </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" t="s">
+        <v>261</v>
+      </c>
+      <c r="C56" t="s">
+        <v>296</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3858,10 +3875,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD56"/>
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4518,6 +4535,20 @@
         <v>86</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>262</v>
+      </c>
+      <c r="B57" t="s">
+        <v>261</v>
+      </c>
+      <c r="C57" t="s">
+        <v>296</v>
+      </c>
+      <c r="D57" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4526,10 +4557,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5172,6 +5203,20 @@
         <v>86</v>
       </c>
     </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" t="s">
+        <v>261</v>
+      </c>
+      <c r="C56" t="s">
+        <v>296</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5182,7 +5227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add mib for new Zmtel
</commit_message>
<xml_diff>
--- a/src/main/resources/SNMP/MibHolder.xlsx
+++ b/src/main/resources/SNMP/MibHolder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spuser.AIRSPAN\git\Testspan_Runners\src\main\resources\SNMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TestSpan\airspan.testspan.jsystem.tests\src\main\resources\SNMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,9 +21,6 @@
     <sheet name="UE" sheetId="7" r:id="rId7"/>
     <sheet name="POWER_CONTROL" sheetId="8" r:id="rId8"/>
   </sheets>
-  <definedNames>
-    <definedName name="ManrCfg_nghRemoveThreshold" localSheetId="2">ENODEB_R15_50!$C$52</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="260">
   <si>
     <t>OID</t>
   </si>
@@ -537,6 +534,9 @@
     <t>pmpDevCpeCellSelectionStartStopLte</t>
   </si>
   <si>
+    <t>1.3.6.1.4.1.17713.20.2.3.1.1.0</t>
+  </si>
+  <si>
     <t>Gemtek start(0) / stop(1) RF</t>
   </si>
   <si>
@@ -807,149 +807,17 @@
     <t xml:space="preserve"> dlEarfcn for ZEMTEL</t>
   </si>
   <si>
-    <t>.1.3.6.1.4.1.17713.20.2.3.1.1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pmpDevCpeLteBandCommit </t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.17713.20.2.3.1.2.15.0</t>
-  </si>
-  <si>
-    <t>commit</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.1.1.3.40</t>
-  </si>
-  <si>
-    <t>asLteStkCellCfgCellId</t>
-  </si>
-  <si>
-    <t>Cell ID for Cell1</t>
-  </si>
-  <si>
-    <t>nghRemoveThreshold</t>
-  </si>
-  <si>
-    <t>asLteStkCellAnrCfgNghRemoveThresholdCell1</t>
-  </si>
-  <si>
-    <t>asLteStkCellAnrCfgNghRemoveThresholdCell2</t>
-  </si>
-  <si>
-    <t>1.3.6.1.4.1.989.1.20.1.4.23.1.33.40</t>
-  </si>
-  <si>
-    <t>1.3.6.1.4.1.989.1.20.1.4.23.1.33.41</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.1.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.2.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.3.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.4.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.5.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.6.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.7.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.8.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.9.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.10.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.11.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.12.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.13.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.14.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.15.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.16.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.17.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.18.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.19.40.174</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.989.1.20.1.4.75.1.20.40.174</t>
-  </si>
-  <si>
-    <t>1.3.6.1.4.1.989.1.20.1.4.1.1.16.40</t>
-  </si>
-  <si>
-    <t>1.3.6.1.4.1.989.1.20.1.4.1.1.16.41</t>
-  </si>
-  <si>
-    <t>asLteStkCellCfgTxPowerCell1</t>
-  </si>
-  <si>
-    <t>asLteStkCellCfgTxPowerCell2</t>
-  </si>
-  <si>
-    <t>Remark #3</t>
-  </si>
-  <si>
-    <t>Zmtel</t>
-  </si>
-  <si>
-    <t>Gemtek</t>
-  </si>
-  <si>
-    <t>PCI</t>
-  </si>
-  <si>
-    <t>pmpDevCpeLtePCID.0</t>
-  </si>
-  <si>
-    <t>pmpDevCpeLtePCID.1</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.17713.20.2.1.2.18.0</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.4.1.17713.20.2.1.2.18.1</t>
-  </si>
-  <si>
-    <t>PCI Cell1</t>
-  </si>
-  <si>
-    <t>PCI Cell2</t>
+    <t>.1.3.6.1.4.1.17713.20.2.3.1.1</t>
+  </si>
+  <si>
+    <t>INTEGER {start ( 0 ) , stop ( 1 ) }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,42 +844,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD3E9FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1020,7 +867,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1034,9 +881,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1320,10 +1164,608 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,86 +1975,86 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1621,7 +2063,7 @@
         <v>102</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>269</v>
+        <v>103</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>104</v>
@@ -1635,7 +2077,7 @@
         <v>105</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>270</v>
+        <v>106</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>107</v>
@@ -1649,7 +2091,7 @@
         <v>108</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>271</v>
+        <v>109</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>110</v>
@@ -1663,7 +2105,7 @@
         <v>111</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>272</v>
+        <v>112</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>113</v>
@@ -1677,7 +2119,7 @@
         <v>114</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>273</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>116</v>
@@ -1691,7 +2133,7 @@
         <v>117</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>274</v>
+        <v>118</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>119</v>
@@ -1705,7 +2147,7 @@
         <v>120</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>275</v>
+        <v>121</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>122</v>
@@ -1719,7 +2161,7 @@
         <v>123</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>276</v>
+        <v>124</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>125</v>
@@ -1733,7 +2175,7 @@
         <v>126</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>277</v>
+        <v>127</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>128</v>
@@ -1747,7 +2189,7 @@
         <v>129</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>278</v>
+        <v>130</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>131</v>
@@ -1761,7 +2203,7 @@
         <v>132</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>279</v>
+        <v>133</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>134</v>
@@ -1775,7 +2217,7 @@
         <v>135</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>280</v>
+        <v>136</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>137</v>
@@ -1789,7 +2231,7 @@
         <v>138</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>281</v>
+        <v>139</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>140</v>
@@ -1803,7 +2245,7 @@
         <v>141</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>282</v>
+        <v>142</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>143</v>
@@ -1817,7 +2259,7 @@
         <v>144</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>283</v>
+        <v>145</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>146</v>
@@ -1831,7 +2273,7 @@
         <v>147</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>284</v>
+        <v>148</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>149</v>
@@ -1845,7 +2287,7 @@
         <v>150</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>285</v>
+        <v>151</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>152</v>
@@ -1859,7 +2301,7 @@
         <v>153</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>286</v>
+        <v>154</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>155</v>
@@ -1873,7 +2315,7 @@
         <v>156</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>287</v>
+        <v>157</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>158</v>
@@ -1887,7 +2329,7 @@
         <v>159</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>288</v>
+        <v>160</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>161</v>
@@ -1910,46 +2352,17 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B52" t="s">
-        <v>267</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B53" t="s">
-        <v>268</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2536,699 +2949,17 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B52" t="s">
-        <v>267</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B53" t="s">
-        <v>268</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B52" t="s">
-        <v>267</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B53" t="s">
-        <v>268</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B54" t="s">
-        <v>289</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="B55" t="s">
-        <v>290</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3815,76 +3546,6 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B52" t="s">
-        <v>267</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B53" t="s">
-        <v>268</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B54" t="s">
-        <v>289</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="B55" t="s">
-        <v>290</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>262</v>
-      </c>
-      <c r="B56" t="s">
-        <v>261</v>
-      </c>
-      <c r="C56" t="s">
-        <v>296</v>
-      </c>
-      <c r="D56" t="s">
-        <v>86</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3893,15 +3554,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -4189,29 +3850,29 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="D31" s="9" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>86</v>
@@ -4219,13 +3880,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>86</v>
@@ -4233,13 +3894,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>86</v>
@@ -4247,13 +3908,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>86</v>
@@ -4261,13 +3922,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>86</v>
@@ -4275,13 +3936,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>86</v>
@@ -4289,13 +3950,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>86</v>
@@ -4303,13 +3964,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>86</v>
@@ -4317,13 +3978,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>86</v>
@@ -4331,13 +3992,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>86</v>
@@ -4345,13 +4006,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>86</v>
@@ -4359,13 +4020,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>86</v>
@@ -4373,13 +4034,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>86</v>
@@ -4387,13 +4048,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>86</v>
@@ -4401,13 +4062,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>86</v>
@@ -4415,13 +4076,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>86</v>
@@ -4429,13 +4090,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>86</v>
@@ -4443,13 +4104,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>86</v>
@@ -4457,13 +4118,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>86</v>
@@ -4471,119 +4132,34 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D52" s="5" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B53" t="s">
-        <v>267</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B54" t="s">
-        <v>268</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B55" t="s">
-        <v>289</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="B56" t="s">
-        <v>290</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>262</v>
-      </c>
-      <c r="B57" t="s">
-        <v>261</v>
-      </c>
-      <c r="C57" t="s">
-        <v>296</v>
-      </c>
-      <c r="D57" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -5165,76 +4741,6 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B52" t="s">
-        <v>267</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B53" t="s">
-        <v>268</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B54" t="s">
-        <v>289</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="B55" t="s">
-        <v>290</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>262</v>
-      </c>
-      <c r="B56" t="s">
-        <v>261</v>
-      </c>
-      <c r="C56" t="s">
-        <v>296</v>
-      </c>
-      <c r="D56" t="s">
-        <v>86</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5243,10 +4749,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5254,10 +4760,10 @@
     <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5270,610 +4776,477 @@
       <c r="D1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>166</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="E7" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E8" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E9" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E14" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E15" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>250</v>
-      </c>
       <c r="D36" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="E36" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" t="s">
-        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Mib name & Oid for new Zemtel device
</commit_message>
<xml_diff>
--- a/src/main/resources/SNMP/MibHolder.xlsx
+++ b/src/main/resources/SNMP/MibHolder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TestSpan\airspan.testspan.jsystem.tests\src\main\resources\SNMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spuser.AIRSPAN\git\Testspan_Runners\src\main\resources\SNMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="260">
   <si>
     <t>OID</t>
   </si>
@@ -807,13 +807,10 @@
     <t xml:space="preserve"> dlEarfcn for ZEMTEL</t>
   </si>
   <si>
-    <t>.1.3.6.1.4.1.17713.20.2.3.1.1</t>
-  </si>
-  <si>
-    <t>INTEGER {start ( 0 ) , stop ( 1 ) }</t>
-  </si>
-  <si>
-    <t>pmpDevCpeCellSelectionStartStopLteZmtel</t>
+    <t>.1.3.6.1.4.1.55686.30.2.1.0</t>
+  </si>
+  <si>
+    <t>lteEnableNew</t>
   </si>
 </sst>
 </file>
@@ -870,7 +867,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -884,7 +881,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4755,7 +4751,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4875,14 +4871,14 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>260</v>
+      <c r="A10" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="B10" t="s">
         <v>258</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>259</v>
+      <c r="C10" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
add remark on MIB_Holder > Power_Control sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/SNMP/MibHolder.xlsx
+++ b/src/main/resources/SNMP/MibHolder.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spuser.AIRSPAN\git\Testspan_Runners\src\main\resources\SNMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sitshakov\git\Testspan_Runners\src\main\resources\SNMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ENODEB_R15_00" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="276">
   <si>
     <t>OID</t>
   </si>
@@ -811,12 +811,63 @@
   </si>
   <si>
     <t>lteEnableNew</t>
+  </si>
+  <si>
+    <t>port 1</t>
+  </si>
+  <si>
+    <t>port 2</t>
+  </si>
+  <si>
+    <t>port 3</t>
+  </si>
+  <si>
+    <t>port 4</t>
+  </si>
+  <si>
+    <t>port 5</t>
+  </si>
+  <si>
+    <t>port 6</t>
+  </si>
+  <si>
+    <t>port 7</t>
+  </si>
+  <si>
+    <t>port 8</t>
+  </si>
+  <si>
+    <t>1 - OFF, 2 - ON</t>
+  </si>
+  <si>
+    <t>2 - OFF, 2 - ON</t>
+  </si>
+  <si>
+    <t>3 - OFF, 2 - ON</t>
+  </si>
+  <si>
+    <t>4 - OFF, 2 - ON</t>
+  </si>
+  <si>
+    <t>5 - OFF, 2 - ON</t>
+  </si>
+  <si>
+    <t>6 - OFF, 2 - ON</t>
+  </si>
+  <si>
+    <t>7 - OFF, 2 - ON</t>
+  </si>
+  <si>
+    <t>8 - OFF, 2 - ON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -867,7 +918,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -881,6 +932,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4750,7 +4807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -5258,15 +5315,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="12"/>
+    <col min="4" max="4" width="23.28515625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5279,7 +5337,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5290,6 +5348,12 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
+      <c r="C2" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5298,6 +5362,12 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
+      <c r="C3" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -5306,6 +5376,12 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
+      <c r="C4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -5314,6 +5390,12 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
+      <c r="C5" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -5322,6 +5404,12 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -5330,6 +5418,12 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -5338,6 +5432,12 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
+      <c r="C8" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -5346,6 +5446,12 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
+      <c r="C9" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5413,5 +5519,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>